<commit_message>
currency progress, asset update kolom, import update
</commit_message>
<xml_diff>
--- a/public/template/TemplateLowValueAsset.xlsx
+++ b/public/template/TemplateLowValueAsset.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Asset Number</t>
   </si>
@@ -35,18 +35,6 @@
     <t>Detail</t>
   </si>
   <si>
-    <t>Pareto</t>
-  </si>
-  <si>
-    <t>Unit No</t>
-  </si>
-  <si>
-    <t>Sn Chassis</t>
-  </si>
-  <si>
-    <t>Sn Engine</t>
-  </si>
-  <si>
     <t>PO No.</t>
   </si>
   <si>
@@ -65,30 +53,15 @@
     <t>Acquisition Value</t>
   </si>
   <si>
-    <t>Production Year</t>
-  </si>
-  <si>
     <t>(Opsional)</t>
   </si>
   <si>
     <t>Kawasaki KLX 150G (Required)</t>
   </si>
   <si>
-    <t>L.Plant-HIM 1057 (Opsional)</t>
-  </si>
-  <si>
     <t>KLX1034 (Opsional)</t>
   </si>
   <si>
-    <t>LX150CEWY2098 (Opsional)</t>
-  </si>
-  <si>
-    <t>MH4LX150GNJP96951 (Opsional)</t>
-  </si>
-  <si>
-    <t>2022 (Opsional)</t>
-  </si>
-  <si>
     <t>EBB202212008 (Opsional)</t>
   </si>
   <si>
@@ -114,6 +87,15 @@
   </si>
   <si>
     <t>HRGA (Required)</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>1057453 (Opsional)</t>
   </si>
 </sst>
 </file>
@@ -491,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,23 +487,20 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" customWidth="1"/>
-    <col min="14" max="14" width="20.44140625" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -530,60 +509,51 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>19</v>
@@ -592,22 +562,13 @@
         <v>20</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>